<commit_message>
Final draft dump 1
</commit_message>
<xml_diff>
--- a/example/Multiple Turbines/Multiple Turbines.xlsx
+++ b/example/Multiple Turbines/Multiple Turbines.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>Berlin</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>rho</t>
-  </si>
-  <si>
-    <t>Anzahl der Stunden mit Flaute</t>
   </si>
   <si>
     <t>Enercon E-70 (2300 kW)</t>
@@ -401,13 +398,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S32"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -442,31 +439,25 @@
         <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="R1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19">
+    </row>
+    <row r="2" spans="1:17">
       <c r="B2">
         <v>0</v>
       </c>
@@ -491,8 +482,8 @@
       <c r="J2">
         <v>1.225</v>
       </c>
-      <c r="K2">
-        <v>533.3842788362903</v>
+      <c r="L2">
+        <v>0</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -507,16 +498,10 @@
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
         <v>1.225</v>
       </c>
-      <c r="S2">
-        <v>533.3842788362903</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19">
+    </row>
+    <row r="3" spans="1:17">
       <c r="B3">
         <v>1</v>
       </c>
@@ -538,11 +523,14 @@
       <c r="I3">
         <v>0</v>
       </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
       <c r="M3">
-        <v>1</v>
+        <v>0.06088861630551259</v>
       </c>
       <c r="N3">
-        <v>0.06088861630551259</v>
+        <v>0</v>
       </c>
       <c r="O3">
         <v>0</v>
@@ -550,11 +538,8 @@
       <c r="P3">
         <v>0</v>
       </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19">
+    </row>
+    <row r="4" spans="1:17">
       <c r="B4">
         <v>2</v>
       </c>
@@ -571,28 +556,28 @@
         <v>3</v>
       </c>
       <c r="H4">
-        <v>0.002912461350106354</v>
+        <v>0.00288333673660529</v>
       </c>
       <c r="I4">
         <v>0.0005437671028695901</v>
       </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
       <c r="M4">
+        <v>0.110824252287152</v>
+      </c>
+      <c r="N4">
         <v>2</v>
       </c>
-      <c r="N4">
-        <v>0.110824252287152</v>
-      </c>
       <c r="O4">
-        <v>2</v>
+        <v>0.001883391673068776</v>
       </c>
       <c r="P4">
-        <v>0.001883391673068776</v>
-      </c>
-      <c r="Q4">
         <v>0.0008300670670641753</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:17">
       <c r="B5">
         <v>3</v>
       </c>
@@ -609,28 +594,28 @@
         <v>48.50000000000001</v>
       </c>
       <c r="H5">
-        <v>0.06036053716162549</v>
+        <v>0.05975693179000923</v>
       </c>
       <c r="I5">
         <v>0.01126953132573957</v>
       </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
       <c r="M5">
-        <v>3</v>
+        <v>0.1420715933757602</v>
       </c>
       <c r="N5">
-        <v>0.1420715933757602</v>
+        <v>18</v>
       </c>
       <c r="O5">
-        <v>18</v>
+        <v>0.02172979337818517</v>
       </c>
       <c r="P5">
-        <v>0.02172979337818517</v>
-      </c>
-      <c r="Q5">
         <v>0.009576970162531903</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:17">
       <c r="B6">
         <v>4</v>
       </c>
@@ -647,28 +632,28 @@
         <v>155</v>
       </c>
       <c r="H6">
-        <v>0.2064312524046646</v>
+        <v>0.204366939880618</v>
       </c>
       <c r="I6">
         <v>0.03854146392628578</v>
       </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
       <c r="M6">
-        <v>4</v>
+        <v>0.1520336223336755</v>
       </c>
       <c r="N6">
-        <v>0.1520336223336755</v>
+        <v>56</v>
       </c>
       <c r="O6">
-        <v>56</v>
+        <v>0.07234416535884763</v>
       </c>
       <c r="P6">
-        <v>0.07234416535884763</v>
-      </c>
-      <c r="Q6">
         <v>0.03188423842863167</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:17">
       <c r="B7">
         <v>5</v>
       </c>
@@ -685,28 +670,28 @@
         <v>339.0000000000001</v>
       </c>
       <c r="H7">
-        <v>0.4253628807988816</v>
+        <v>0.4211092519908928</v>
       </c>
       <c r="I7">
         <v>0.07941679341146428</v>
       </c>
+      <c r="L7">
+        <v>5</v>
+      </c>
       <c r="M7">
-        <v>5</v>
+        <v>0.1432371872681138</v>
       </c>
       <c r="N7">
-        <v>0.1432371872681138</v>
+        <v>127</v>
       </c>
       <c r="O7">
-        <v>127</v>
+        <v>0.1545736085121363</v>
       </c>
       <c r="P7">
-        <v>0.1545736085121363</v>
-      </c>
-      <c r="Q7">
         <v>0.06812521457851303</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:17">
       <c r="B8">
         <v>6</v>
       </c>
@@ -723,28 +708,28 @@
         <v>627.5</v>
       </c>
       <c r="H8">
-        <v>0.6687648946334147</v>
+        <v>0.6620772456870806</v>
       </c>
       <c r="I8">
         <v>0.1248608326570305</v>
       </c>
+      <c r="L8">
+        <v>6</v>
+      </c>
       <c r="M8">
-        <v>6</v>
+        <v>0.1216621904406874</v>
       </c>
       <c r="N8">
-        <v>0.1216621904406874</v>
+        <v>240</v>
       </c>
       <c r="O8">
-        <v>240</v>
+        <v>0.2481091115070262</v>
       </c>
       <c r="P8">
-        <v>0.2481091115070262</v>
-      </c>
-      <c r="Q8">
         <v>0.1093491096118991</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:17">
       <c r="B9">
         <v>7</v>
       </c>
@@ -761,28 +746,28 @@
         <v>1035.5</v>
       </c>
       <c r="H9">
-        <v>0.8558303908694835</v>
+        <v>0.8472720869607887</v>
       </c>
       <c r="I9">
         <v>0.1597866396317514</v>
       </c>
+      <c r="L9">
+        <v>7</v>
+      </c>
       <c r="M9">
-        <v>7</v>
+        <v>0.09434817306062671</v>
       </c>
       <c r="N9">
-        <v>0.09434817306062671</v>
+        <v>400</v>
       </c>
       <c r="O9">
-        <v>400</v>
+        <v>0.3206781184523029</v>
       </c>
       <c r="P9">
-        <v>0.3206781184523029</v>
-      </c>
-      <c r="Q9">
         <v>0.1413324424556065</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:17">
       <c r="B10">
         <v>8</v>
       </c>
@@ -799,28 +784,28 @@
         <v>1549</v>
       </c>
       <c r="H10">
-        <v>0.9133232487777113</v>
+        <v>0.9041900162899342</v>
       </c>
       <c r="I10">
         <v>0.1705207648345831</v>
       </c>
+      <c r="L10">
+        <v>8</v>
+      </c>
       <c r="M10">
-        <v>8</v>
+        <v>0.06730835689970192</v>
       </c>
       <c r="N10">
-        <v>0.06730835689970192</v>
+        <v>626</v>
       </c>
       <c r="O10">
-        <v>626</v>
+        <v>0.3580297889753402</v>
       </c>
       <c r="P10">
-        <v>0.3580297889753402</v>
-      </c>
-      <c r="Q10">
         <v>0.1577944413294184</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:17">
       <c r="B11">
         <v>9</v>
       </c>
@@ -837,28 +822,28 @@
         <v>2090</v>
       </c>
       <c r="H11">
-        <v>0.812695628090271</v>
+        <v>0.8045686718093682</v>
       </c>
       <c r="I11">
         <v>0.1517332228924827</v>
       </c>
+      <c r="L11">
+        <v>9</v>
+      </c>
       <c r="M11">
-        <v>9</v>
+        <v>0.04438922178291227</v>
       </c>
       <c r="N11">
-        <v>0.04438922178291227</v>
+        <v>892</v>
       </c>
       <c r="O11">
-        <v>892</v>
+        <v>0.3364482130377158</v>
       </c>
       <c r="P11">
-        <v>0.3364482130377158</v>
-      </c>
-      <c r="Q11">
         <v>0.1482827950280532</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:17">
       <c r="B12">
         <v>10</v>
       </c>
@@ -875,28 +860,28 @@
         <v>2580</v>
       </c>
       <c r="H12">
-        <v>0.6136593089238449</v>
+        <v>0.6075227158346065</v>
       </c>
       <c r="I12">
         <v>0.1145724198366748</v>
       </c>
+      <c r="L12">
+        <v>10</v>
+      </c>
       <c r="M12">
-        <v>10</v>
+        <v>0.02715210563005933</v>
       </c>
       <c r="N12">
-        <v>0.02715210563005933</v>
+        <v>1223</v>
       </c>
       <c r="O12">
-        <v>1223</v>
+        <v>0.2821667344067622</v>
       </c>
       <c r="P12">
-        <v>0.2821667344067622</v>
-      </c>
-      <c r="Q12">
         <v>0.1243593231303111</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:17">
       <c r="B13">
         <v>11</v>
       </c>
@@ -913,28 +898,28 @@
         <v>2900</v>
       </c>
       <c r="H13">
-        <v>0.3922647377705748</v>
+        <v>0.388342090392869</v>
       </c>
       <c r="I13">
-        <v>0.07323725000079945</v>
+        <v>0.07323725000079946</v>
+      </c>
+      <c r="L13">
+        <v>11</v>
       </c>
       <c r="M13">
-        <v>11</v>
+        <v>0.01544106194971559</v>
       </c>
       <c r="N13">
-        <v>0.01544106194971559</v>
+        <v>1590</v>
       </c>
       <c r="O13">
-        <v>1590</v>
+        <v>0.2086172086426061</v>
       </c>
       <c r="P13">
-        <v>0.2086172086426061</v>
-      </c>
-      <c r="Q13">
         <v>0.09194384630305183</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:17">
       <c r="B14">
         <v>12</v>
       </c>
@@ -951,28 +936,28 @@
         <v>3000</v>
       </c>
       <c r="H14">
-        <v>0.2149238075087078</v>
+        <v>0.2127745694336207</v>
       </c>
       <c r="I14">
-        <v>0.04012705478218408</v>
+        <v>0.04012705478218409</v>
+      </c>
+      <c r="L14">
+        <v>12</v>
       </c>
       <c r="M14">
-        <v>12</v>
+        <v>0.008178227074151743</v>
       </c>
       <c r="N14">
-        <v>0.008178227074151743</v>
+        <v>1900</v>
       </c>
       <c r="O14">
-        <v>1900</v>
+        <v>0.1320348590795162</v>
       </c>
       <c r="P14">
-        <v>0.1320348590795162</v>
-      </c>
-      <c r="Q14">
         <v>0.05819171327639375</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:17">
       <c r="B15">
         <v>13</v>
       </c>
@@ -989,28 +974,28 @@
         <v>3000</v>
       </c>
       <c r="H15">
-        <v>0.1061579549418479</v>
+        <v>0.1050963753924294</v>
       </c>
       <c r="I15">
         <v>0.01982007541599863</v>
       </c>
+      <c r="L15">
+        <v>13</v>
+      </c>
       <c r="M15">
-        <v>13</v>
+        <v>0.004039496002353421</v>
       </c>
       <c r="N15">
-        <v>0.004039496002353421</v>
+        <v>2080</v>
       </c>
       <c r="O15">
-        <v>2080</v>
+        <v>0.07139476329689078</v>
       </c>
       <c r="P15">
-        <v>0.07139476329689078</v>
-      </c>
-      <c r="Q15">
         <v>0.03146580853096247</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:17">
       <c r="B16">
         <v>14</v>
       </c>
@@ -1027,28 +1012,28 @@
         <v>3000</v>
       </c>
       <c r="H16">
-        <v>0.0489503285839764</v>
+        <v>0.04846082529813664</v>
       </c>
       <c r="I16">
-        <v>0.009139203978673002</v>
+        <v>0.009139203978673004</v>
+      </c>
+      <c r="L16">
+        <v>14</v>
       </c>
       <c r="M16">
-        <v>14</v>
+        <v>0.001862645684321781</v>
       </c>
       <c r="N16">
-        <v>0.001862645684321781</v>
+        <v>2230</v>
       </c>
       <c r="O16">
-        <v>2230</v>
+        <v>0.03529481858666646</v>
       </c>
       <c r="P16">
-        <v>0.03529481858666646</v>
-      </c>
-      <c r="Q16">
         <v>0.01555548267825783</v>
       </c>
     </row>
-    <row r="17" spans="2:17">
+    <row r="17" spans="2:16">
       <c r="B17">
         <v>15</v>
       </c>
@@ -1065,28 +1050,28 @@
         <v>3000</v>
       </c>
       <c r="H17">
-        <v>0.02108869433857283</v>
+        <v>0.0208778073951871</v>
       </c>
       <c r="I17">
-        <v>0.003937335760136121</v>
+        <v>0.003937335760136122</v>
+      </c>
+      <c r="L17">
+        <v>15</v>
       </c>
       <c r="M17">
-        <v>15</v>
+        <v>0.0008024617328224059</v>
       </c>
       <c r="N17">
-        <v>0.0008024617328224059</v>
+        <v>2300</v>
       </c>
       <c r="O17">
-        <v>2300</v>
+        <v>0.01568295902311866</v>
       </c>
       <c r="P17">
-        <v>0.01568295902311866</v>
-      </c>
-      <c r="Q17">
         <v>0.006911949322785593</v>
       </c>
     </row>
-    <row r="18" spans="2:17">
+    <row r="18" spans="2:16">
       <c r="B18">
         <v>16</v>
       </c>
@@ -1103,28 +1088,28 @@
         <v>3000</v>
       </c>
       <c r="H18">
-        <v>0.008494185597444959</v>
+        <v>0.00840924374147051</v>
       </c>
       <c r="I18">
         <v>0.001585895274933203</v>
       </c>
+      <c r="L18">
+        <v>16</v>
+      </c>
       <c r="M18">
-        <v>16</v>
+        <v>0.0003232186300397625</v>
       </c>
       <c r="N18">
-        <v>0.0003232186300397625</v>
+        <v>2310</v>
       </c>
       <c r="O18">
-        <v>2310</v>
+        <v>0.006344307222731639</v>
       </c>
       <c r="P18">
-        <v>0.006344307222731639</v>
-      </c>
-      <c r="Q18">
         <v>0.002796126033809118</v>
       </c>
     </row>
-    <row r="19" spans="2:17">
+    <row r="19" spans="2:16">
       <c r="B19">
         <v>17</v>
       </c>
@@ -1141,28 +1126,28 @@
         <v>3000</v>
       </c>
       <c r="H19">
-        <v>0.003200416405957113</v>
+        <v>0.003168412241897542</v>
       </c>
       <c r="I19">
-        <v>0.0005975293567346587</v>
+        <v>0.0005975293567346588</v>
+      </c>
+      <c r="L19">
+        <v>17</v>
       </c>
       <c r="M19">
-        <v>17</v>
+        <v>0.000121781446193193</v>
       </c>
       <c r="N19">
-        <v>0.000121781446193193</v>
+        <v>2310</v>
       </c>
       <c r="O19">
-        <v>2310</v>
+        <v>0.002390391013609367</v>
       </c>
       <c r="P19">
-        <v>0.002390391013609367</v>
-      </c>
-      <c r="Q19">
         <v>0.001053516847385378</v>
       </c>
     </row>
-    <row r="20" spans="2:17">
+    <row r="20" spans="2:16">
       <c r="B20">
         <v>18</v>
       </c>
@@ -1179,28 +1164,28 @@
         <v>3000</v>
       </c>
       <c r="H20">
-        <v>0.001128491644627742</v>
+        <v>0.001117206728181465</v>
       </c>
       <c r="I20">
-        <v>0.0002106934851476598</v>
+        <v>0.0002106934851476599</v>
+      </c>
+      <c r="L20">
+        <v>18</v>
       </c>
       <c r="M20">
-        <v>18</v>
+        <v>4.294108236787451E-05</v>
       </c>
       <c r="N20">
-        <v>4.294108236787451E-05</v>
+        <v>2310</v>
       </c>
       <c r="O20">
-        <v>2310</v>
+        <v>0.0008428704093724606</v>
       </c>
       <c r="P20">
-        <v>0.0008428704093724606</v>
-      </c>
-      <c r="Q20">
         <v>0.0003714782106278488</v>
       </c>
     </row>
-    <row r="21" spans="2:17">
+    <row r="21" spans="2:16">
       <c r="B21">
         <v>19</v>
       </c>
@@ -1217,28 +1202,28 @@
         <v>3000</v>
       </c>
       <c r="H21">
-        <v>0.0003725290911097837</v>
+        <v>0.0003688038001986859</v>
       </c>
       <c r="I21">
-        <v>6.955253315207479E-05</v>
+        <v>6.95525331520748E-05</v>
+      </c>
+      <c r="L21">
+        <v>19</v>
       </c>
       <c r="M21">
-        <v>19</v>
+        <v>1.417538398439055E-05</v>
       </c>
       <c r="N21">
-        <v>1.417538398439055E-05</v>
+        <v>2310</v>
       </c>
       <c r="O21">
-        <v>2310</v>
+        <v>0.0002782419781498974</v>
       </c>
       <c r="P21">
-        <v>0.0002782419781498974</v>
-      </c>
-      <c r="Q21">
         <v>0.0001226295656074008</v>
       </c>
     </row>
-    <row r="22" spans="2:17">
+    <row r="22" spans="2:16">
       <c r="B22">
         <v>20</v>
       </c>
@@ -1255,28 +1240,28 @@
         <v>3000</v>
       </c>
       <c r="H22">
-        <v>0.000115167465541118</v>
+        <v>0.0001140157908857068</v>
       </c>
       <c r="I22">
         <v>2.150218373879545E-05</v>
       </c>
+      <c r="L22">
+        <v>20</v>
+      </c>
       <c r="M22">
-        <v>20</v>
+        <v>4.382323650727474E-06</v>
       </c>
       <c r="N22">
-        <v>4.382323650727474E-06</v>
+        <v>2310</v>
       </c>
       <c r="O22">
-        <v>2310</v>
+        <v>8.601858001266104E-05</v>
       </c>
       <c r="P22">
-        <v>8.601858001266104E-05</v>
-      </c>
-      <c r="Q22">
         <v>3.791096214617664E-05</v>
       </c>
     </row>
-    <row r="23" spans="2:17">
+    <row r="23" spans="2:16">
       <c r="B23">
         <v>21</v>
       </c>
@@ -1293,28 +1278,28 @@
         <v>3000</v>
       </c>
       <c r="H23">
-        <v>3.335222435351769E-05</v>
+        <v>3.301870210998251E-05</v>
       </c>
       <c r="I23">
-        <v>6.226981316097684E-06</v>
+        <v>6.226981316097685E-06</v>
+      </c>
+      <c r="L23">
+        <v>21</v>
       </c>
       <c r="M23">
-        <v>21</v>
+        <v>1.269110515735072E-06</v>
       </c>
       <c r="N23">
-        <v>1.269110515735072E-06</v>
+        <v>2310</v>
       </c>
       <c r="O23">
-        <v>2310</v>
+        <v>2.491077636964236E-05</v>
       </c>
       <c r="P23">
-        <v>2.491077636964236E-05</v>
-      </c>
-      <c r="Q23">
         <v>1.097892455144433E-05</v>
       </c>
     </row>
-    <row r="24" spans="2:17">
+    <row r="24" spans="2:16">
       <c r="B24">
         <v>22</v>
       </c>
@@ -1331,28 +1316,28 @@
         <v>3000</v>
       </c>
       <c r="H24">
-        <v>9.049953702796485E-06</v>
+        <v>8.959454165768521E-06</v>
       </c>
       <c r="I24">
         <v>1.689659196986035E-06</v>
       </c>
+      <c r="L24">
+        <v>22</v>
+      </c>
       <c r="M24">
-        <v>22</v>
+        <v>3.44366579254052E-07</v>
       </c>
       <c r="N24">
-        <v>3.44366579254052E-07</v>
+        <v>2310</v>
       </c>
       <c r="O24">
-        <v>2310</v>
+        <v>6.759410420618695E-06</v>
       </c>
       <c r="P24">
-        <v>6.759410420618695E-06</v>
-      </c>
-      <c r="Q24">
         <v>2.979074434253961E-06</v>
       </c>
     </row>
-    <row r="25" spans="2:17">
+    <row r="25" spans="2:16">
       <c r="B25">
         <v>23</v>
       </c>
@@ -1369,28 +1354,28 @@
         <v>3000</v>
       </c>
       <c r="H25">
-        <v>2.301347245690364E-06</v>
+        <v>2.27833377323346E-06</v>
       </c>
       <c r="I25">
         <v>4.296698819506267E-07</v>
       </c>
+      <c r="L25">
+        <v>23</v>
+      </c>
       <c r="M25">
-        <v>23</v>
+        <v>8.757029093190122E-08</v>
       </c>
       <c r="N25">
-        <v>8.757029093190122E-08</v>
+        <v>2310</v>
       </c>
       <c r="O25">
-        <v>2310</v>
+        <v>1.718876257806133E-06</v>
       </c>
       <c r="P25">
-        <v>1.718876257806133E-06</v>
-      </c>
-      <c r="Q25">
         <v>7.575602007619582E-07</v>
       </c>
     </row>
-    <row r="26" spans="2:17">
+    <row r="26" spans="2:16">
       <c r="B26">
         <v>24</v>
       </c>
@@ -1407,28 +1392,28 @@
         <v>3000</v>
       </c>
       <c r="H26">
-        <v>5.48540468144118E-07</v>
+        <v>5.430550634626768E-07</v>
       </c>
       <c r="I26">
         <v>1.024144959583974E-07</v>
       </c>
+      <c r="L26">
+        <v>24</v>
+      </c>
       <c r="M26">
-        <v>24</v>
+        <v>2.087292496743219E-08</v>
       </c>
       <c r="N26">
-        <v>2.087292496743219E-08</v>
+        <v>2310</v>
       </c>
       <c r="O26">
-        <v>2310</v>
+        <v>4.097048756568417E-07</v>
       </c>
       <c r="P26">
-        <v>4.097048756568417E-07</v>
-      </c>
-      <c r="Q26">
         <v>1.805691983039517E-07</v>
       </c>
     </row>
-    <row r="27" spans="2:17">
+    <row r="27" spans="2:16">
       <c r="B27">
         <v>25</v>
       </c>
@@ -1445,28 +1430,28 @@
         <v>3000</v>
       </c>
       <c r="H27">
-        <v>1.225724950067493E-07</v>
+        <v>1.213467700566818E-07</v>
       </c>
       <c r="I27">
         <v>2.288472961156497E-08</v>
       </c>
+      <c r="L27">
+        <v>25</v>
+      </c>
       <c r="M27">
-        <v>25</v>
+        <v>4.664097983514053E-09</v>
       </c>
       <c r="N27">
-        <v>4.664097983514053E-09</v>
+        <v>2310</v>
       </c>
       <c r="O27">
-        <v>2310</v>
+        <v>9.154939652054106E-08</v>
       </c>
       <c r="P27">
-        <v>9.154939652054106E-08</v>
-      </c>
-      <c r="Q27">
         <v>4.034855847986205E-08</v>
       </c>
     </row>
-    <row r="28" spans="2:17">
+    <row r="28" spans="2:16">
       <c r="B28">
         <v>26</v>
       </c>
@@ -1488,11 +1473,14 @@
       <c r="I28">
         <v>0</v>
       </c>
+      <c r="L28">
+        <v>26</v>
+      </c>
       <c r="M28">
-        <v>26</v>
+        <v>9.771676129241713E-10</v>
       </c>
       <c r="N28">
-        <v>9.771676129241713E-10</v>
+        <v>0</v>
       </c>
       <c r="O28">
         <v>0</v>
@@ -1500,11 +1488,8 @@
       <c r="P28">
         <v>0</v>
       </c>
-      <c r="Q28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:17">
+    </row>
+    <row r="29" spans="2:16">
       <c r="B29">
         <v>27</v>
       </c>
@@ -1526,11 +1511,14 @@
       <c r="I29">
         <v>0</v>
       </c>
+      <c r="L29">
+        <v>27</v>
+      </c>
       <c r="M29">
-        <v>27</v>
+        <v>1.919729386733474E-10</v>
       </c>
       <c r="N29">
-        <v>1.919729386733474E-10</v>
+        <v>0</v>
       </c>
       <c r="O29">
         <v>0</v>
@@ -1538,11 +1526,8 @@
       <c r="P29">
         <v>0</v>
       </c>
-      <c r="Q29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:17">
+    </row>
+    <row r="30" spans="2:16">
       <c r="B30">
         <v>28</v>
       </c>
@@ -1564,11 +1549,14 @@
       <c r="I30">
         <v>0</v>
       </c>
+      <c r="L30">
+        <v>28</v>
+      </c>
       <c r="M30">
-        <v>28</v>
+        <v>3.536936685308475E-11</v>
       </c>
       <c r="N30">
-        <v>3.536936685308475E-11</v>
+        <v>0</v>
       </c>
       <c r="O30">
         <v>0</v>
@@ -1576,11 +1564,8 @@
       <c r="P30">
         <v>0</v>
       </c>
-      <c r="Q30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:17">
+    </row>
+    <row r="31" spans="2:16">
       <c r="B31">
         <v>29</v>
       </c>
@@ -1602,11 +1587,14 @@
       <c r="I31">
         <v>0</v>
       </c>
+      <c r="L31">
+        <v>29</v>
+      </c>
       <c r="M31">
-        <v>29</v>
+        <v>6.111850610988651E-12</v>
       </c>
       <c r="N31">
-        <v>6.111850610988651E-12</v>
+        <v>0</v>
       </c>
       <c r="O31">
         <v>0</v>
@@ -1614,11 +1602,8 @@
       <c r="P31">
         <v>0</v>
       </c>
-      <c r="Q31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:17">
+    </row>
+    <row r="32" spans="2:16">
       <c r="B32">
         <v>30</v>
       </c>
@@ -1640,19 +1625,19 @@
       <c r="I32">
         <v>0</v>
       </c>
+      <c r="L32">
+        <v>30</v>
+      </c>
       <c r="M32">
-        <v>30</v>
+        <v>9.906356171995162E-13</v>
       </c>
       <c r="N32">
-        <v>9.906356171995162E-13</v>
+        <v>0</v>
       </c>
       <c r="O32">
         <v>0</v>
       </c>
       <c r="P32">
-        <v>0</v>
-      </c>
-      <c r="Q32">
         <v>0</v>
       </c>
     </row>

</xml_diff>